<commit_message>
pruebas con la grafica
</commit_message>
<xml_diff>
--- a/pruebas.xlsx
+++ b/pruebas.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SCIS2PC15\Documents\numerosAmigos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ser\Documents\numerosAmigos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C18D20-1508-4C5D-A1D8-8D5D62853923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -68,7 +80,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,6 +169,892 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.1706036745406825E-2"/>
+          <c:y val="9.7638888888888886E-2"/>
+          <c:w val="0.8966272965879265"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$E$4:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.7299999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1585</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.24310000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.28649999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4259</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5171</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65939999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3359999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.2677</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3A85-4AA4-8AC4-BAE0EC7844EB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="917247840"/>
+        <c:axId val="1088136624"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="917247840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1088136624"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1088136624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="917247840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent5"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CD82E48-9E85-C58A-303E-607184091C71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -421,14 +1319,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
@@ -600,5 +1501,28 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{BBA1B68E-015D-4C1B-8003-0F0EECBE46FB}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Hoja1!E4:E13</xm:f>
+              <xm:sqref>I5</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>